<commit_message>
done import product with header
</commit_message>
<xml_diff>
--- a/public/data_file/Product1.xlsx
+++ b/public/data_file/Product1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Horotononeoh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F26C1A4-CCE5-44DB-B7A3-0DCCB4044554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27713AF0-F81E-4F85-81F5-87156FFD4829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>BULLET PAYMENT</t>
   </si>
@@ -44,16 +44,58 @@
   </si>
   <si>
     <t>Dummy 6</t>
+  </si>
+  <si>
+    <t>PARTNER</t>
+  </si>
+  <si>
+    <t>DEBITUR</t>
+  </si>
+  <si>
+    <t>NILAI_PEMBIAYAAN_POKOK_MAXIMUM</t>
+  </si>
+  <si>
+    <t>SUKU_BUNGA_FLAT</t>
+  </si>
+  <si>
+    <t>JANGKA_WAKTU_MAXIMUM</t>
+  </si>
+  <si>
+    <t>POLA_PEMBAYARAN</t>
+  </si>
+  <si>
+    <t>BIAYA_ADMINISTRASI</t>
+  </si>
+  <si>
+    <t>BIAYA_ASURANSI</t>
+  </si>
+  <si>
+    <t>BIAYA_PROVINSI</t>
+  </si>
+  <si>
+    <t>BIAYA_LAIN_LAIN</t>
+  </si>
+  <si>
+    <t>JENIS_PRODUK</t>
+  </si>
+  <si>
+    <t>SUKU_BUNGA_EFFECTIVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,14 +118,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -94,6 +180,40 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{745E31F1-CFFF-49C9-A7AB-DA62776C5553}" name="Table2" displayName="Table2" ref="A1:L3" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:L3" xr:uid="{745E31F1-CFFF-49C9-A7AB-DA62776C5553}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{C6665516-7062-42C8-888F-F2B87B04500B}" name="PARTNER"/>
+    <tableColumn id="2" xr3:uid="{C77D0DA4-45ED-46EB-89D3-FDE7A714E3E0}" name="DEBITUR"/>
+    <tableColumn id="3" xr3:uid="{384DF41D-838B-4FFA-9642-A241829A351B}" name="JENIS_PRODUK"/>
+    <tableColumn id="4" xr3:uid="{7706F106-21B8-4172-99FC-2FE831455FF5}" name="NILAI_PEMBIAYAAN_POKOK_MAXIMUM" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5C136AE0-2BE0-4F54-A1E5-8BC226749505}" name="SUKU_BUNGA_FLAT" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{85F6C0BE-5432-49B6-923C-D5F1666F9C5F}" name="SUKU_BUNGA_EFFECTIVE" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FEE8CD6B-C8B4-407C-8590-0B879EC82DA2}" name="JANGKA_WAKTU_MAXIMUM" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{501E1ABC-499B-4534-AE89-E8A1332FDCF7}" name="POLA_PEMBAYARAN"/>
+    <tableColumn id="9" xr3:uid="{4B4F5EE1-E892-47D0-8F16-7281432E86A7}" name="BIAYA_ADMINISTRASI" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{FF94BCE8-CAD9-476D-BE45-F1CC05AB0410}" name="BIAYA_ASURANSI" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{DB214B79-D7A1-49D1-8428-BC7A21328B28}" name="BIAYA_PROVINSI" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{99D02BF3-D116-43ED-8026-CAA99A23C921}" name="BIAYA_LAIN_LAIN" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,10 +513,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:N2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -415,84 +537,125 @@
     <col min="14" max="14" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:14">
-      <c r="C1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G1" s="1">
+      <c r="D2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="H1" s="1">
+      <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="I1" s="1">
+      <c r="G2" s="1">
         <v>190909</v>
       </c>
-      <c r="J1" t="s">
+      <c r="H2" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L1" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M1" s="1">
-        <v>10000</v>
-      </c>
-      <c r="N1" s="1">
+      <c r="I2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L2" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="3:14">
-      <c r="C2" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1">
+      <c r="D3" s="1">
         <v>100000</v>
       </c>
-      <c r="G2" s="1">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
+      <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="1">
+      <c r="G3" s="1">
         <v>1222</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="I3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L3" s="1">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>